<commit_message>
Check for NA in formula values.
Closes #31
</commit_message>
<xml_diff>
--- a/tests/testthat/missing-values.xlsx
+++ b/tests/testthat/missing-values.xlsx
@@ -19,13 +19,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -463,36 +467,50 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f>A2</f>
+        <v>NA</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B4" si="0">A3</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>